<commit_message>
Adding FS GS line
</commit_message>
<xml_diff>
--- a/Lineindicator/stop.xlsx
+++ b/Lineindicator/stop.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludwig/Documents/Personal/Apps/SubwayConnect/Lineindicator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0C9AC51D-395B-EF4F-96D0-3902D0946EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B72EB8-C3EC-514B-A2B5-2EAFC3633347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="520" windowWidth="28040" windowHeight="17540" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="1860" yWindow="520" windowWidth="28040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stop" sheetId="1" r:id="rId1"/>
-    <sheet name="42nd St" sheetId="13" r:id="rId2"/>
-    <sheet name="Flushing" sheetId="12" r:id="rId3"/>
-    <sheet name="Dyre Avenue" sheetId="10" r:id="rId4"/>
-    <sheet name="Pelham" sheetId="11" r:id="rId5"/>
-    <sheet name="Lexington Avenue" sheetId="9" r:id="rId6"/>
-    <sheet name="Jerome Avenue" sheetId="8" r:id="rId7"/>
-    <sheet name="Lenox Avenue " sheetId="4" r:id="rId8"/>
-    <sheet name="New Lots" sheetId="7" r:id="rId9"/>
-    <sheet name="Eastern Parkway" sheetId="5" r:id="rId10"/>
-    <sheet name="Nostrand Avenue" sheetId="6" r:id="rId11"/>
-    <sheet name="White Plains Road" sheetId="3" r:id="rId12"/>
-    <sheet name="Bway_7th Ave" sheetId="2" r:id="rId13"/>
-    <sheet name="Sheet13" sheetId="14" r:id="rId14"/>
+    <sheet name="42nd St" sheetId="13" state="hidden" r:id="rId2"/>
+    <sheet name="Flushing" sheetId="12" state="hidden" r:id="rId3"/>
+    <sheet name="Dyre Avenue" sheetId="10" state="hidden" r:id="rId4"/>
+    <sheet name="Pelham" sheetId="11" state="hidden" r:id="rId5"/>
+    <sheet name="Lexington Avenue" sheetId="9" state="hidden" r:id="rId6"/>
+    <sheet name="Jerome Avenue" sheetId="8" state="hidden" r:id="rId7"/>
+    <sheet name="Lenox Avenue " sheetId="4" state="hidden" r:id="rId8"/>
+    <sheet name="New Lots" sheetId="7" state="hidden" r:id="rId9"/>
+    <sheet name="Eastern Parkway" sheetId="5" state="hidden" r:id="rId10"/>
+    <sheet name="Nostrand Avenue" sheetId="6" state="hidden" r:id="rId11"/>
+    <sheet name="White Plains Road" sheetId="3" state="hidden" r:id="rId12"/>
+    <sheet name="Bway_7th Ave" sheetId="2" state="hidden" r:id="rId13"/>
+    <sheet name="Master" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -5282,7 +5282,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -6132,11 +6132,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1504"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338:B352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12558,10 +12558,10 @@
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A338">
+      <c r="A338" s="2">
         <v>501</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B338" s="2" t="s">
         <v>339</v>
       </c>
       <c r="D338">
@@ -12575,10 +12575,10 @@
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A339" t="s">
+      <c r="A339" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B339" s="2" t="s">
         <v>339</v>
       </c>
       <c r="D339">
@@ -12595,10 +12595,10 @@
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A340" t="s">
+      <c r="A340" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B340" s="2" t="s">
         <v>339</v>
       </c>
       <c r="D340">
@@ -12615,10 +12615,10 @@
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A341">
+      <c r="A341" s="2">
         <v>502</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B341" s="2" t="s">
         <v>342</v>
       </c>
       <c r="D341">
@@ -12632,10 +12632,10 @@
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A342" t="s">
+      <c r="A342" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B342" s="2" t="s">
         <v>342</v>
       </c>
       <c r="D342">
@@ -12652,10 +12652,10 @@
       </c>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A343" t="s">
+      <c r="A343" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B343" s="2" t="s">
         <v>342</v>
       </c>
       <c r="D343">
@@ -12672,10 +12672,10 @@
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A344">
+      <c r="A344" s="2">
         <v>503</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B344" s="2" t="s">
         <v>141</v>
       </c>
       <c r="D344">
@@ -12689,10 +12689,10 @@
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A345" t="s">
+      <c r="A345" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B345" s="2" t="s">
         <v>141</v>
       </c>
       <c r="D345">
@@ -12709,10 +12709,10 @@
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A346" t="s">
+      <c r="A346" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B346" s="2" t="s">
         <v>141</v>
       </c>
       <c r="D346">
@@ -12729,10 +12729,10 @@
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A347">
+      <c r="A347" s="2">
         <v>504</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B347" s="2" t="s">
         <v>150</v>
       </c>
       <c r="D347">
@@ -12746,10 +12746,10 @@
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A348" t="s">
+      <c r="A348" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B348" s="2" t="s">
         <v>150</v>
       </c>
       <c r="D348">
@@ -12766,10 +12766,10 @@
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A349" t="s">
+      <c r="A349" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B349" s="2" t="s">
         <v>150</v>
       </c>
       <c r="D349">
@@ -12786,10 +12786,10 @@
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A350">
+      <c r="A350" s="2">
         <v>505</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B350" s="2" t="s">
         <v>349</v>
       </c>
       <c r="D350">
@@ -12803,10 +12803,10 @@
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A351" t="s">
+      <c r="A351" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B351" s="2" t="s">
         <v>349</v>
       </c>
       <c r="D351">
@@ -12823,10 +12823,10 @@
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A352" t="s">
+      <c r="A352" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B352" s="2" t="s">
         <v>349</v>
       </c>
       <c r="D352">
@@ -34737,7 +34737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -35025,7 +35025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -35216,7 +35216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0"/>
@@ -35719,7 +35719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView topLeftCell="A113" workbookViewId="0">
@@ -36800,10 +36800,10 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -36896,7 +36896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36968,7 +36968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37520,7 +37520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37664,7 +37664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38120,7 +38120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView topLeftCell="A36" workbookViewId="0"/>
@@ -38695,7 +38695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
@@ -39057,7 +39057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -39224,7 +39224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>